<commit_message>
add main info in mail
</commit_message>
<xml_diff>
--- a/OlxScraper/flats.xlsx
+++ b/OlxScraper/flats.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,17 +466,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>562720134</t>
+          <t>556190687</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>! Do wynajęcia mieszkanie 2pok na Złotnikach-Dobra Komunikacja !</t>
+          <t>GRUNWALD dla pan Studentek</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1 200 zł</t>
+          <t>1 100 zł</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Parter</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Szeregowiec</t>
+          <t>Blok</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>35 m²</t>
+          <t>34 m²</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1 zł</t>
+          <t>80 zł</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Fabryczna</t>
+          <t>Śródmieście</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -546,14 +546,22 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Do wynajęcia BEZPOŚREDNIO mieszkanie 2 pokojowe, 35 m2, ul. Rawicka na Złotnikach, w domu jednorodzinnym - osobne wejście. Pełne wyposażenie, internet i tv. Mieszkanie składa się z 2 pokoi, 1 łazienki z WC, kuchni i korytarza. Bardzo przytulne mieszkanie w cichej i spokojnej okolicy, na około niska zabudowa domów jednorodzinnych. Bardzo blisko przystanek autobusowy i tramwajowy - doskonała komunikacja z centrum miasta.
-Proszę o kontakt tylko telefoniczny.</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr"/>
+          <t>GRUNWALD - dwupokojowe mieszkanko dla 2 dziewczyn Studentek. Sztucznie przerobiona kawalerka,  (dwa nieprzechodnie pokoiki po ok 10 m kazdy, scianki dzialowe z plyt gipsowych), dla dwoch 
+dziewczyn lubiacych mieszkac razem, ale jednoczesnie kazda w swoim oddzielnym nieprzechodnim pokoiku. 
+Osobna widna kuchnia, lazienka (WC, wanna z prysznicem, umywalka,  i automatyczna pralka),  oszklony balkon, ciepla woda i ogrzewanie miejskie, gaz miejski, winda, domofon, 1 pietro.  Zamieszkanie 
+bez wlasciciela.  Tylko Wy dwie w calym mieszkaniu. Pelne umeblowanie.  1100 PLN. 
+Ciepla woda, ogrzewanie oraz oplaty do spoldzielni oplacane przez wlasciciela. Kaucja zwrotna po zakonczeniu  zamieszkania. Umowa  do 30 czerwca z mozliwoscia przedluzenia na nastepny rok akademicki. 
+5 minut pieszo do Pasazu Grunwaldzkiego (Rondo Regana). Tramwaje i autobusy w granicach 4 minut.  10 minut tramwajem do Rynku. PW, UW, UP i AM w zasiegu 10 do 15 minut pieszo. Kontakt poprzez email.</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>794-140-116</t>
+        </is>
+      </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/do-wynajecia-mieszkanie-2pok-na-zlotnikach-dobra-komunikacja-CID3-IDC57dc.html#3c151eb37f</t>
+          <t>https://www.olx.pl/oferta/grunwald-dla-pan-studentek-CID3-IDBDIBx.html#a4c335e894</t>
         </is>
       </c>
     </row>
@@ -648,11 +656,7 @@
 Agencjom dziekuję - prosze nie dzwonić.</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>690-433-939</t>
-        </is>
-      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
           <t>https://www.olx.pl/oferta/mieszkanie-41m2-na-maslicach-CID3-IDC5glL.html#3c151eb37f</t>
@@ -662,27 +666,27 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>562739364</t>
+          <t>562791391</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dwupokojowe I 38mkw I Przy UE I Krzyki-Centrum</t>
+          <t>Wynajmę 2 pokoje, 56m2, rozkładowe, ul. Łodzka</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1 350 zł</t>
+          <t>1 400 zł</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Biuro / Deweloper</t>
+          <t>Osoby prywatnej</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -697,7 +701,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>38 m²</t>
+          <t>56 m²</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -707,7 +711,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>350 zł</t>
+          <t>650 zł</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -722,7 +726,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Śródmieście</t>
+          <t>Krzyki</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -742,119 +746,13 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Do wynajęcia od zaraz mieszkanie dwupokojowe nierozkładowe (salon z przejściem do kuchni, sypialnia, łazienka, przedpokój) o powierzchni 38mkw.
-Mieszkanie znajduje się na trzecim piętrze w czteropiętrowym bloku.
-Lokal w pełni wyposażony i umeblowany
-Wszystkie media miejskie
-okna Pcv
-Możliwość podłączenia internetu
-Miejsce świetnie skomunikowane,w pobliżu przystanki tramwajowe i autobusowe .
-Ulica Komandroska!
-Nieopodal Uniwersytet Ekonomiczny.
-Wkoło pełna infrastruktura handlowo-usługowa.
-Cena 1350zł+czynsz 350zł+ liczniki
-Bartłomiej Domowicz
-Fidom Nieruchomości
- 516 - pokaż numer telefonu -</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/dwupokojowe-i-38mkw-i-przy-ue-i-krzyki-centrum-CID3-IDC5cdm.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>562791391</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Wynajmę 2 pokoje, 56m2, rozkładowe, ul. Łodzka</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1 400 zł</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Osoby prywatnej</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>56 m²</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>650 zł</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Krzyki</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
           <t>Wynajmę w pełni rozkładowe mieszkanie na 1 piętrze.
-W skład mieszkania wchodzi:
+Mieszkanie składa się z:
 - przedpokój
 - kuchnia 
 - łazienka
 - osobna toaleta 
-- mały
+- mały pokój 
 - duży pokój
 - balkon (wyjście z obu pokoi).
 Wszystkie pomieszczenia są umeblowane jak na zdjęciach.
@@ -865,31 +763,120 @@
 Świetna lokalizacja, obok aquaparku, 10 min piechotą do dworca PKP/PKS, 2 min do przystanku Gajowa.</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>48 601-968-321</t>
-        </is>
-      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/wynajme-2-pokoje-56m2-rozkladowe-ul-lodzka-CID3-IDC5pKw.html#3c151eb37f</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>562819054</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Wygodne mieszkanie w centrum Wrocławia</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1 400 zł</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parter</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>37 m²</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>380 zł</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Śródmieście</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>października</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2019,</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Wynajmę rozkładowe mieszkanie w centrum Wrocławia przy ul. Pomorskiej - 10 minut na piechotę do Starego Rynku; przystanek tramwajowy bezpośrednio pod blokiem.  Kuchnia w pełni wyposażona. W łazience pralka. Pokoje częściowo umeblowane. Istnie możliwość uzupełnienia wyposażenia. Podany czynsz uwzględnia zużycie wody przy dwóch osobach. Do mieszkania należy miejsce postojowe na ogrodzonym parkingu.  Kaucja zwrotna 1400. Dodatkowe opłaty prąd+gaz ok. 60 zł miesięcznie. Wolne od 1.11.2019r.</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/wynajme-2-pokoje-56m2-rozkladowe-ul-lodzka-CID3-IDC5pKw.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/wygodne-mieszkanie-w-centrum-wroclawia-CID3-IDC5vVG.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>562819054</t>
+          <t>545361671</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wygodne mieszkanie w centrum Wrocławia</t>
+          <t>Mieszkanie do wynajęcia</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1 400 zł</t>
+          <t>1 500 zł</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -899,7 +886,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Parter</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -914,7 +901,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>37 m²</t>
+          <t>50,50 m²</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -924,7 +911,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>380 zł</t>
+          <t>525 zł</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -939,7 +926,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Śródmieście</t>
+          <t>Krzyki</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -959,17 +946,24 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Wynajmę rozkładowe mieszkanie w centrum Wrocławia przy ul. Pomorskiej - 10 minut na piechotę do Starego Rynku; przystanek tramwajowy bezpośrednio pod blokiem.  Kuchnia w pełni wyposażona. W łazience pralka. Pokoje częściowo umeblowane. Istnie możliwość uzupełnienia wyposażenia. Podany czynsz uwzględnia zużycie wody przy dwóch osobach. Do mieszkania należy miejsce postojowe na ogrodzonym parkingu.  Kaucja zwrotna 1400. Dodatkowe opłaty prąd+gaz ok. 60 zł miesięcznie. Wolne od 1.11.2019r.</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>533 774 767</t>
-        </is>
-      </c>
+          <t>mieszkanie przy ul. Gubińskiej 8 o powierzchni 50.5 m składa się z : 
+- duży i mały pokój
+- kuchnia z jadalnią
+- przedpokój
+- łazienka+ osobna toaleta
+- balkon
+Ogrzewanie miejskie, okna PCV, TV kablowa, mieszkanie umeblowane i wyposażone w sprzęt AGD.
+Budynek jest monitorowany i w godzinach nocnych z ochroną.
+Koszt wynajmu to 1500 zł + 700 zł za media tj. czynsz wraz ciepłą i zimną wodą, prąd, gaz i TV kablowa.
+Kaucja 2000 zł
+Jeśli nie odbieram telefonu proszę o sms.
+Pozdrawiam. Marek</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/wygodne-mieszkanie-w-centrum-wroclawia-CID3-IDC5vVG.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/mieszkanie-do-wynajecia-CID3-IDAUhtZ.html#3c151eb37f</t>
         </is>
       </c>
     </row>
@@ -1091,31 +1085,27 @@
 Opis oferty zawarty na stronie internetowej sporządzany jest na podstawie oględzin nieruchomości oraz informacji uzyskanych od właściciela, może podlegać aktualizacji i nie stanowi oferty określonej w art. 66 i następnych K.C.</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>577 147 947</t>
-        </is>
-      </c>
+      <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/przytulne-2-pokojowe-mieszkanie-z-balkonem-na-gaju-CID3-IDC5rdT.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/przytulne-2-pokojowe-mieszkanie-z-balkonem-na-gaju-CID3-IDC5rdT.html#3c151eb37f</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>545361671</t>
+          <t>562794490</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mieszkanie do wynajęcia</t>
+          <t>2 pokojowe Mieszkanie Muchobór Wielki Wrocław</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1 500 zł</t>
+          <t>1 600 zł</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1125,7 +1115,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>Parter</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1140,7 +1130,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>50,50 m²</t>
+          <t>44 m²</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1150,7 +1140,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>510 zł</t>
+          <t>400 zł</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1165,7 +1155,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Krzyki</t>
+          <t>Fabryczna</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1185,45 +1175,30 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>mieszkanie przy ul. Gubińskiej 8 o powierzchni 50.5 m składa się z : 
-- duży i mały pokój
-- kuchnia z jadalnią
-- przedpokój
-- łazienka+ osobna toaleta
-- balkon
-Ogrzewanie miejskie, okna PCV, TV kablowa, mieszkanie umeblowane i wyposażone w sprzęt AGD.
-Budynek jest monitorowany i w godzinach nocnych z ochroną.
-Koszt wynajmu to 1500 zł + 700 zł za media tj. czynsz wraz ciepłą i zimną wodą, prąd, gaz i TV kablowa.
-Kaucja 2000 zł
-Jeśli nie odbieram telefonu proszę o sms.
-Pozdrawiam. Marek</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>501 466 414</t>
-        </is>
-      </c>
+          <t>Słoneczne 2 pokoje z aneksem kuchennym i balkonem, windą, osiedle zamknięte, umeblowane i wyposażone w telewizor, lodówkę, płytę indukcyjną, piekarnik, pralkę, garnki oraz zastawę, sztućce, a także czajnik elektryczny. Lokalizacja ul. Krzemieniecka w sąsiedztwie STOKROTKI i NETTO. W pobliżu przystanek autobusowy linii 107, 119, 319. Niedaleko mieszkania centrum handlowe Factoria. Do ceny wynajmu 1600zł. należy doliczyć czynsz 400 liczniki wody, prądu, ogrzewania około 200zł. Kaucja zwrotna 2000zł. Kontakt telefoniczny 691 -661412 Wynajmu możliwy od zaraz.</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-do-wynajecia-CID3-IDAUhtZ.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/2-pokojowe-mieszkanie-muchobor-wielki-wroclaw-CID3-IDC5qyu.html#3c151eb37f</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>505156690</t>
+          <t>548448010</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mieszkanie 2-pokojowe, ul. M. Hłaski, Muchobór Wielki, OD 1 LISTOPADA</t>
+          <t>Dwupokojowe na Zalesiu</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1 550 zł</t>
+          <t>1 700 zł</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1233,7 +1208,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Parter</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1243,12 +1218,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Blok</t>
+          <t>Dom wolnostojący</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>48 m²</t>
+          <t>34 m²</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1258,7 +1233,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>380 zł</t>
+          <t>1 zł</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1273,12 +1248,12 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Fabryczna</t>
+          <t>Śródmieście</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1293,37 +1268,36 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Witam,
-do wynajęcia mieszkanie 2-pokojowe, oddzielna kuchnia wyposażona w kuchenkę gazową, lodówkę i mikrofalówkę.  Mieszkanie w pełni umeblowane. W przedpokoju szafa wnękowa. Internet i telewizja w cenie najmu.
-Mieszkanie dla osób niepalących. Dostępne od 1 listopada.
-Opłaty:
-- najem 1550 zł;
--czynsz 380 zł + woda + ogrzewanie; 
--dodatkowo prąd, gaz.
-Kaucja zwrotna 1550 zł.</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr"/>
+          <t>Wynajmę dwupokojowe mieszkanie przy ulicy Noskowskiego na Zalesiu. 
+W najbliższym sąsiedztwie placu Grunwaldzkiego i większości wrocławskich uczelni. W bezpośrednim sąsiedztwie są korty tenisowe, kryty basen, park szczytnicki, Stadion Olimpijski, Morskie Oko - kąpielisko i bulwary nad Odrą. 
+Opłata miesięczna 1700,- zł zawiera ogrzewanie, internet, wywóz śmieci.</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>48 726 903 271</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-2-pokojowe-ul-m-hlaski-muchobor-wielki-od-1-listopada-CID3-IDybAky.html#3c151eb37f</t>
+          <t>https://www.olx.pl/oferta/dwupokojowe-na-zalesiu-CID3-IDB7enE.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>562794490</t>
+          <t>562783920</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2 pokojowe Mieszkanie Muchobór Wielki Wrocław</t>
+          <t>Wynajmę mieszkanie KOZANÓW 50m2 FLAT FOR RENT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1 600 zł</t>
+          <t>1 700 zł</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1333,7 +1307,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Parter</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1348,7 +1322,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>44 m²</t>
+          <t>50 m²</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1358,7 +1332,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>400 zł</t>
+          <t>470 zł</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1392,103 +1366,6 @@
         </is>
       </c>
       <c r="Q10" t="inlineStr">
-        <is>
-          <t>Słoneczne 2 pokoje z aneksem kuchennym i balkonem, windą, osiedle zamknięte, umeblowane i wyposażone w telewizor, lodówkę, płytę indukcyjną, piekarnik, pralkę, garnki oraz zastawę, sztućce, a także czajnik elektryczny. Lokalizacja ul. Krzemieniecka w sąsiedztwie STOKROTKI i NETTO. W pobliżu przystanek autobusowy linii 107, 119, 319. Niedaleko mieszkania centrum handlowe Factoria. Do ceny wynajmu 1600zł. należy doliczyć czynsz 400 liczniki wody, prądu, ogrzewania około 200zł. Kaucja zwrotna 2000zł. Kontakt telefoniczny 691 -661412 Wynajmu możliwy od zaraz.</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>785808453</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/2-pokojowe-mieszkanie-muchobor-wielki-wroclaw-CID3-IDC5qyu.html#a4c335e894</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>562783920</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Wynajmę mieszkanie KOZANÓW 50m2 FLAT FOR RENT</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1 700 zł</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Osoby prywatnej</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>50 m²</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>470 zł</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Fabryczna</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
         <is>
           <t>ZAPRASZAM DO KONTAKTU/ WE SPEAK ENGLISH!
 Witam! Do wynajęcia mam przestronne mieszkanie w zielonej części dzielnicy Kozanów na ulicy Gwareckiej, przy samym wale. 2 pokoje, w tym jeden z aneksem kuchennym, łazienka z wanną, duży przedpokój i balkon z ławką. Nowe budownictwo, budynek poza blokowiskiem, doskonałe połączenie z centrum miasta - pod samym blokiem przystanki tramwajów 31 i 32, autobusy 101, 102, 103, 104, 132, 136, nocny 245. Doskonały i szybki dojazd do rynku! Tramwajem (zawsze bez korków!) zajmuje to ok. 15 min. Obok przystanku znajduje się również wypożyczalnia rowerów miejskich.
@@ -1503,99 +1380,95 @@
 https://photos.app.goo.gl/BdiqBmUwruBafBas6</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>575 925 123</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/wynajme-mieszkanie-kozanow-50m2-flat-for-rent-CID3-IDC5nO0.html#a4c335e894</t>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/wynajme-mieszkanie-kozanow-50m2-flat-for-rent-CID3-IDC5nO0.html#3c151eb37f</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>559784686</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Rozkład | 2-pok | Od zaraz | okolice Kruczej</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>1 790 zł</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Biuro / Deweloper</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Blok</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>48 m²</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>2 pokoje</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>500 zł</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Wrocław,</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Dolnośląskie,</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>Krzyki</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>października</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>2019,</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Do wynajęcia 2-pokojowe mieszkanie na I piętrze w bloku przy ul. Stalowowolskiej.
 Mieszkanie jest jasne, przestronne i w pełni rozkładowe z osobną kuchnią. Idealne dla 2-3 osób - studentów bądź grupy znajomych. W pobliżu Centrum Handlowe Borek, sklepy, restauracje i wszystkie niezbędne punkty usługowo-handlowe oraz przystanki komunikacji miejskiej.
@@ -1628,22 +1501,124 @@
 Niniejsza oferta nie stanowi oferty w rozumieniu przepisów Kodeksu Cywilnego, a dane w niej zawarte mają jedynie charakter informacyjny i mogą ulec zmianie.</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/rozklad-2-pok-od-zaraz-okolice-kruczej-CID3-IDBSNzg.html#3c151eb37f</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>518022394</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mieszkanie 2-Pokoje Zielony Taras Duży Parking Wrocław Krzyki Brochów</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1 800 zł</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Parter</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>46 m²</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>200 zł</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Krzyki</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>października</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2019,</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Wynajmę mieszkanie we Wrocławiu dzielnica Krzyki osiedle Brochów.Mieszkanie rozkładowe 2-pokojowe z aneksem kuchennym,garderoba,zielony taras 40 m2,duży parking ze szlabanem.Dobra komunikacja do centrum miasta,autobusy 114,125,133,325 lub pociągiem ze stacji PKP 5-min do centrum miasta na Dworzec Główny.W pobliżu szkoła,przedszkole,żłobek,szpital,przychodnia,kościół,Fresh,Biedronka,apteka,Dworzec PKP,duży park Brochowski.
+Dodatkowe opłaty;
+Opłaty administracyjne,zaliczka na wodę i ogrzewanie 200 zł.
+Opłaty za energię elektryczną według zużycia.
+Wymagana kaucja 2000 zł.
+Mieszkanie do zamieszkania od zaraz.</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>577 503 403</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/rozklad-2-pok-od-zaraz-okolice-kruczej-CID3-IDBSNzg.html#3c151eb37f</t>
+          <t>https://www.olx.pl/oferta/mieszkanie-2-pokoje-zielony-taras-duzy-parking-wroclaw-krzyki-brochow-CID3-IDz3zhU.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>526660447</t>
+          <t>562775996</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Mieszkanie, PL. Grunwaldzki, 2 Pokoje</t>
+          <t>Złotnicka, pelne umeblowanie, ciche, komfortowe</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1653,12 +1628,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Osoby prywatnej</t>
+          <t>Biuro / Deweloper</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1673,7 +1648,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>38 m²</t>
+          <t>50 m²</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1683,7 +1658,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>550 zł</t>
+          <t>400 zł</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1698,7 +1673,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Śródmieście</t>
+          <t>Fabryczna</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1717,125 +1692,6 @@
         </is>
       </c>
       <c r="Q13" t="inlineStr">
-        <is>
-          <t>FOR ENGLISH: CALL ME OR SEND AN E-MAIL
-Mam do wynajęcia urządzone, przytulne, jasne, z pięknym widokiem, 2 pokojowe mieszkanie w centrum Wrocławia przy Placu Grunwaldzkim.
-Mieszkanie dostępne od 01.11.2019, wyposażenie widoczne na zdjęciach należy na aktualnych najemców.
-Lokal funkcjonalnie dopasowany dla jednej osoby lub pary. Nie wynajmuję pokoi osobno.
-    Lokalizacja: Pl. Grunwaldzki,
-    Ilość pokoi: 2,
-    Metraż: 38 m2,
-    Piętro: 9/15,
-    2 windy,
-    Domofon,
-    Internet,
-    Telewizja osiedlowa,
-LOKAL SKŁADA SIĘ Z:
-    Pokój dzienny,
-    Pokój mały,
-    Kuchnia,
-    Łazienka,
-    Przedpokój,
-    Dwa niezależne balkony,
-    Komórka lokatorska,
-OPIS NIERUCHOMOŚCI:
-Mieszkanie na 9 piętrze z dwoma windami w budynku. Posiada piękny widok na stronę zachodnią i Most Grunwaldzki, idealne dla osób ceniących bliskość Centrum. Niedaleko międzynarodowe korporacje: Credit Suisse, DataArt, HPE oraz Uczelnie PWR, UP, UW, UM. Do Wrocławskiego Rynku ok 10 min spacerem. W pobliżu liczne punkty handlowo – usługowe, Pasaż Grunwaldzki. Bardzo dobra komunikacja miejska w każdym kierunku miasta.
-WYPOSAŻENIE:
-Kuchnia z meblami w zabudowie z osobnym balkonem, wyposażona w sprzęt AGD (kuchenka gazowa, piekarnik, lodówka, mikrofalówka, czajnik). Pokój duży w pełni wyposażony z osobnym balkonem (meble, rozkładane łóżko, dywan, stolik, 2 krzesła, telewizor). Pokój mały (meble, dywan, łóżko), łazienka (prysznic, WC, pralka, umywalka), przedpokój (wieszak, dywan, lustro),
-Cena najmu:  1800 zł,
-Opłaty dodatkowe: 550 zł ( czynsz administracyjny, prąd, gaz, internet),
-Kaucja: cena najmu + opłaty dodatkowe,</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-pl-grunwaldzki-2-pokoje-CID3-IDzDOrl.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>562775996</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Złotnicka, pelne umeblowanie, ciche, komfortowe</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1 800 zł</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Biuro / Deweloper</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>50 m²</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>400 zł</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Fabryczna</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
         <is>
           <t>Polecam do wynajęcia komfortowe 2-pokojowe,  mieszkanie  o powierzchni 50m2 położone w budynku  z 2009r., w dzielnicy Fabryczna przy ul. Złotnickiej, na 2 piętrze w 3- piętrowym budynku. Mieszkanie składa się z przestronnego salonu z wyjściem na balkon, częściowo otwartej  kuchni, dużej  sypialni, łazienki i przedpokoju.   Kuchnia zabudowana jest meblami na wymiar wraz ze sprzętem AGD (lodówka z zamrażarką, piekarnik, płyta ceramiczna, zmywarka, okap) obok kuchnia jadalnia wyposażona w stół z krzesłami.   Łazienka z wanną  wykończona w jasnej  glazurze, wyposażona w pralkę. Sypialnia posiada rozkładaną wersalkę, biurko oraz przestronną szafę wnękową typu Komandor.  W salonie wygodny komplet wypoczynkowy, komoda pod RTV, szafa. Mieszkanie  wykończone zostało z materiałów wysokiej jakości,  jest jasne, przestronne  i słoneczne.  W pobliżu przystanek  autobusowy i tramwajowy, szybki dojazd do Centrum miasta oraz wyjazd na obwodnicę miasta. Budynek położony w cichym, zielonym otoczeniu.  
 Opłaty: 1800 zł/mies. + opłata administracyjna 400 zł+ energia elektryczna. 
@@ -1843,41 +1699,146 @@
 KONTAKT: Actiwa Nieruchomości, Anna Leszko tel.  501 - pokaż numer telefonu - ,</t>
         </is>
       </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/zlotnicka-pelne-umeblowanie-ciche-komfortowe-CID3-IDC5lKc.html#3c151eb37f</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>562873902</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2 pokojowe mieszkanie dla pary na Grabiszynie</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1 900 zł</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>37,60 m²</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>425 zł</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Fabryczna</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>października</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2019,</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Do wynajęcia 2-pokojowe świeżo wyremontowane mieszkanie o powierzchni 37 m2 mieszczące się na 1. piętrze budynku przy Alei Pracy, na Grabiszynie. 
+Mieszkanie składa się z sypialni, salonu z aneksem kuchennym, łazienki i przedpokoju. Mieszkanie słoneczne. Ogrzewanie i woda miejskie.
+Pełne umeblowanie, m.in.: duża lodówka z zamrażarką i dystrybutorem wody, płyta gazowa, okap, zmywarka, kuchenka mikrofalowa, piekarnik, płaski telewizor, pojemna pralka, sofa 3 osobowa, stolik kawowy, meble RTV, stół z krzesłami, łóżko dwuosobowe, 2 pojemne szafy w zabudowie, w łazience wanna z prysznicem.
+Osiedle ogrodzone szlabanami, dostępne są bezpłatne miejsca postojowe pod samym budynkiem dla mieszkańców.
+Idealne dla singla lub pracującej pary, maksymalnie dla dwóch osób.
+Spokojna okolica, w pobliżu ul. Grabiszyńska, 
+Świetny dojazd do każdej części miasta:
+linie tramwajowe (14, 4, 5, 11, 20, 24), 
+linie autobusowe (136, 126, 119, 125, 134, 124).
+W pobliżu sklepy:, BIEDRONKA, LIDL, SPOŁEM, ŻABKA, ROSSMANN oraz centrum handlowe Tarasy Grabiszyńskie.
+Najem: 1900,00 PLN + 425 PLN (czynsz administracyjny) + prąd i gaz wg zużycia
+Wymagana jest kaucja zwrotna: 2300zł
+Pośrednikom serdecznie dziękujemy :)</t>
+        </is>
+      </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>2250-230</t>
+          <t>733 999 437</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/zlotnicka-pelne-umeblowanie-ciche-komfortowe-CID3-IDC5lKc.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/2-pokojowe-mieszkanie-dla-pary-na-grabiszynie-CID3-IDC5Ldk.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>562747613</t>
+          <t>556103051</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2 pok. mieszkanie, 40m2, garaż w cenie! Bajana! Lokum da Vinci</t>
+          <t>Wynajmę</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1 800 zł</t>
+          <t>1 900 zł</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Biuro / Deweloper</t>
+          <t>Osoby prywatnej</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1887,12 +1848,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Apartamentowiec</t>
+          <t>Kamienica</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>40 m²</t>
+          <t>56 m²</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1902,7 +1863,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>450 zł</t>
+          <t>10 zł</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1922,7 +1883,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1937,51 +1898,34 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Do wynajęcia w pełni wyposażone 2-pokojowe mieszkanie, przy ul. Bajana, Drzewieckiego o powierzchni 40m2 położony na osiedlu Lokum da Vinci.
-Nieruchomość znajduje się na 10 piętrze budynku.
-Mieszkanie składa się z:
-` salonu z aneksem kuchennym
-` sypialni
-` łazienki z WC
-` przedpokoju
-` dodatkowo: balkonu
-Kuchnia w zabudowie, sprzęt AGD (zmywarka, piekarnik, lodówka, zamrażarka, okap, płyta grzewcza). Łazienka z WC, wanną, pralką. 
-W cenie najmu!: miejsce postojowe w garażu podziemnymi komórka lokatorska
-Mieszkanie bardzo ciche, a jednocześnie oddalone 10-15 min tramwajem od rynku.
-Okolica:
-W pobliżu znajdują się liczne punkty usługowe, gastronomiczne, sklepy, apteki, kawiarnia, Hala Targowa Tęcza.
-Cena:
-1800zł czynsz najmu + opłaty czynszowe 450zł + prąd wg zużycia
-Wymagana kaucja zwrotna
-Zapraszamy na prezentację !
-Doctor House Estates
-Paula Wolańczyk
-+ 486 - pokaż numer telefonu - 
-+ 488 - pokaż numer telefonu - 
-Ogłoszenie nie stanowi oferty w rozumieniu przepisów Kodeksu Cywilnego, a dane w nim zawarte mają charakter informacyjny i mogą ulec zmianie.</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr"/>
+          <t>Wynajmę mieszkanie w centrum miasta,5 min do rynku,PL.Dubois.Mieszkanie składa się z kuchni,łazienki,p.pokoju,salonu 25m2,małego pokoju 12 m2.ogrzewanie gazowe,do mieszkania przynależna piwnica.Opłaty 1900 najem plus  ,prąd,gaz,woda wg.stanu licznika/ ok. 300 zł/.Mieszkanie dla max.4 osób,kaucja 800 zł.</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>501 466 414</t>
+        </is>
+      </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/2-pok-mieszkanie-40m2-garaz-w-cenie-bajana-lokum-da-vinci-CID3-IDC5emp.html#3c151eb37f</t>
+          <t>https://www.olx.pl/oferta/wynajme-CID3-IDBDlO3.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>559281475</t>
+          <t>562811333</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2 pokoje Gaj</t>
+          <t>Idealne dla pary / przestronne / balkon / Gaj</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1 800 zł</t>
+          <t>1 900 zł</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1991,7 +1935,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2006,7 +1950,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>43 m²</t>
+          <t>52 m²</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2016,7 +1960,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>500 zł</t>
+          <t>270 zł</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -2050,112 +1994,6 @@
         </is>
       </c>
       <c r="Q16" t="inlineStr">
-        <is>
-          <t>Na wynajem jasne, przytulne mieszkanie na ul. Piławskiej we Wrocławiu.
-Czteropiętrowy blok mieszkalny z windą, oddany do użytku w 2003 roku.
-Budynek przystosowany dla osób niepełnosprawnych.
-Linie tramwajowe 31,32, linie autobusowe miejskie: 145, 146, K.
-Odległość od centrum Wrocławia około 5,5 km
-Mieszkanie w pełni umeblowane.
-Jeden z pokoi niedawno był odmalowywany.
-Do mieszkania przynależy balkon.
-Do wynajęcia od zaraz.
-Ogrzewanie miejskie.
-Koszty: 1800+ ok 500zł opłat(wszystkie)
-Obowiązuje kaucja
-internet we własnym zakresie
-Kontakt:  785 - pokaż numer telefonu -  lub  785 - pokaż numer telefonu -</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/2-pokoje-gaj-CID3-IDBQGEX.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>562811333</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Idealne dla pary / przestronne / balkon / Gaj</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1 900 zł</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Biuro / Deweloper</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>52 m²</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>270 zł</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Krzyki</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
         <is>
           <t>Do wynajęcia 2 pokojowe mieszkanie przy ul.Wandy Rutkiewicz niedaleko Ferio Gaj.
 Mieszkanie ciepłe i przytulne, w pełni wyposażone, przeznaczone dla 2 osób. Atrakcyjna lokalizacja, osiedle ciche i bezpieczne z dużym patio oraz placami zabaw. W pobliżu wiele sklepów, siłownie, piekarnia, cukiernia, warzywniak, placówki oświatowe itd.
@@ -2193,201 +2031,95 @@
 Opis oferty zawarty na stronie internetowej sporządzany jest na podstawie oględzin nieruchomości oraz informacji uzyskanych od właściciela, może podlegać aktualizacji i nie stanowi oferty określonej w art. 66 i następnych K.C.</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>883-010-777</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/idealne-dla-pary-przestronne-balkon-gaj-CID3-IDC5uV9.html#a4c335e894</t>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/idealne-dla-pary-przestronne-balkon-gaj-CID3-IDC5uV9.html#3c151eb37f</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>558738711</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2pok. NOWE Bud, 2017r, Krzyki/OŁTASZYN, OGRÓDEK</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>545062256</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Mieszkanie wynajem 1 900 zł</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>1 900 zł</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Biuro / Deweloper</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Parter</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Apartamentowiec</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>47 m²</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>42 m²</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>2 pokoje</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>350 zł</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>500 zł</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>Wrocław,</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>Dolnośląskie,</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Krzyki</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Fabryczna</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>18:26,</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>Do wynajęcia od ZARAZ, dwupokojowe mieszkanie w budynku z 2017r. Nieruchomość składa się z przestronnego salonu połączonego z wyposażonym w niezbędne sprzęty AGD aneksem kuchennym, drugiego, w pełni umeblowanego pokoju, łazienki z wanną oraz pralką, a także przedpokoju z zabudowaną szafą. Z salonu wyjście na OGRÓDEK.
-Mieszkanie znajduje się na parterze. Przynależne miejsce postojowe w GARAŻU PODZIEMNYM W CENIE!.
-Bardzo dobra lokalizacja, o okolicy nowe osiedla oraz wille. W pobliżu mieszkania Fresh Market.
-Tuż przy osiedlu przystanek linii 113.
-Cena: 1900 zł + opłaty administracyjne 350 zł + prąd wg wskazań rachunków
-Kaucja: 2300 zł
-Zapraszam na prezentację,
-Weronika Burlińska
-Fidom Nieruchomości
- 512 - pokaż numer telefonu -</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/2pok-nowe-bud-2017r-krzyki-oltaszyn-ogrodek-CID3-IDBOpsH.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>545062256</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Mieszkanie wynajem 1 900 zł</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>1 900 zł</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Osoby prywatnej</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>42 m²</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>500 zł</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Fabryczna</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>18:26,</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>Lokalizacja: ul. Na Ostatnim Groszu 106, Fabryczna 
 • Ilość pokoi: 2
@@ -2402,37 +2134,233 @@
 Kaucja w wysokości 2000zł.</t>
         </is>
       </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/mieszkanie-wynajem-1-900-zl-CID3-IDAT1AI.html#3c151eb37f</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>562806451</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Przytulne mieszkanie Przy ul.Klasztorna od teraz.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1 900 zł
+Do negocjacji</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>45 m²</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>500 zł</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Krzyki</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>18:37,</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Wynajmę umeblowane mieszkanie po remoncie w budynku 2011r. W cenie miejsce postojowe w podziemnym garażu. Miesięczna kaucja 2400 zł.
+Kontakt  533 - pokaż numer telefonu -</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/przytulne-mieszkanie-przy-ul-klasztorna-od-teraz-CID3-IDC5tFp.html#3c151eb37f</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>559972747</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ŁADNE CZYSTE 2-pokojowe mieszkanko na Biskupinie OD ZARAZ z ogrodkiem!</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1 900 zł
+Do negocjacji</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Biuro / Deweloper</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Kamienica</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>50 m²</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>100 zł</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Śródmieście</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>października</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>2019,</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>DO WYNAJĘCIA OD ZARAZ bardzo ładne CZYSTE 2-pokojowe mieszkanko na Biskupinie, w jednej z cichych uliczek blisko Parku Biskupińskiego.
+Mieszkanie o powierzchni ok. 50 mkw położone jest na II piętrze kameralnej kamienicy. Posiada jasną dobrze wyposażoną kuchnię (nowa elektryczna płyta grzewcza!), 2 pokoje ze wschodnią orientacją okien, łazienkę z oknem oraz przedpokój.
+Wnętrza bardzo czyste, świeżo po remoncie, ściany odmalowane, wymienione okna i podłogi. 
+Umeblowanie jak na zdjęciach. PIERWSZY NAJEM - możliwość doposażenia np. w biurko, łóżko, oprawy oświetleniowe. 
+Kwota 1.900,- PLN / miesiąc, uśredniona w ciągu roku, obejmuje wszelkie opłaty eksploatacyjne, w tym korzystanie ze stałego łącza internetowego.
+W komórce lokatorskiej miejsce na rower etc. 
+Dostępny dla lokatorów OGRÓD widoczny z okna - jako miejsce na rekreację / suszenie prania.
+W pobliżu przystanki komunikacji miejskiej, sklep, usługi.
+ŚWIETNA OFERTA dla osób ceniących ciszę, czystość i jedną z najlepszych lokalizacji w skali miasta.</t>
+        </is>
+      </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>573 979 567</t>
+          <t>533 774 767</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-wynajem-1-900-zl-CID3-IDAT1AI.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/ladne-czyste-2-pokojowe-mieszkanko-na-biskupinie-od-zaraz-z-ogrodkiem-CID3-IDBTAuw.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>562806451</t>
+          <t>559679582</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Przytulne mieszkanie Przy ul.Klasztorna od teraz.</t>
+          <t>2 pok. ul. Racławicka Wygodne Ciepłe Balkon Jasna Kuchnia M.Parkingowe</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1 900 zł
-Do negocjacji</t>
+          <t>2 000 zł</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Osoby prywatnej</t>
+          <t>Biuro / Deweloper</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2447,12 +2375,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Blok</t>
+          <t>Apartamentowiec</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>45 m²</t>
+          <t>54 m²</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2462,7 +2390,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>500 zł</t>
+          <t>480 zł</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2482,45 +2410,57 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>19</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>18:37,</t>
+          <t>października</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>2019,</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>Wynajmę umeblowane mieszkanie po remoncie w budynku 2011r. W cenie miejsce postojowe w podziemnym garażu. Miesięczna kaucja 2400 zł.
-Kontakt  533 - pokaż numer telefonu -</t>
+          <t>2 pok. KRZYKI ul. Racławicka 
+Nowe Budownictwo Balkon 
+Media Miejskie Dwustronne Domofon 
+5 min spacerem do Parku Górka Skarbowców Relaks i Rekreacja 
+Mieszkanie Ciche i Ciepłe 
+Miejsce Parkingowe w Garażu Podziemnym + 200 zł
+Do wynajęcia mieszkanie 2 pok. o pow 54 m2 położone na I pietrze.
+Mieszkanie w pełni urządzone i wyposażone m.in. zmywarka, pralka, lodówka, szafy w zabudowie.
+Dodatkowe opłaty: czynsz do zarządcy 480 zł w tym ogrzewanie, woda, wywóz śmieci, utrzymanie części wspólnych, prąd w/g zużycia ok 70 zł
+Wymagana kaucja zwrotna.
+Brak zgody na zwierzęta domowe.
+Zapraszam do kontaktu:
+BN Nowe Mieszkania
+Tel. Joanna 575.743.231</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>48 660-335-417</t>
+          <t>785414685</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/przytulne-mieszkanie-przy-ul-klasztorna-od-teraz-CID3-IDC5tFp.html#a4c335e894</t>
+          <t>https://www.olx.pl/oferta/2-pok-ul-raclawicka-wygodne-cieple-balkon-jasna-kuchnia-m-parkingowe-CID3-IDBSme2.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>558822390</t>
+          <t>556935556</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Komfortowe 2 pok, internet, TV sat, wyposażone, ul.Hłaski, Muchobór</t>
+          <t>Mieszkanie do wynajęcia - nowe osiedle</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2550,7 +2490,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>47 m²</t>
+          <t>46,50 m²</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2575,7 +2515,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Fabryczna</t>
+          <t>Krzyki</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2594,211 +2534,6 @@
         </is>
       </c>
       <c r="Q21" t="inlineStr">
-        <is>
-          <t>Bez prowizji! Piękne, jasne 2-pokojowe mieszkanie w doskonałym stanie, składające się z pokoju dziennego i osobnej sypialni.
-Mieszkanie wyposażone w nowy sprzęt i meble, w przedpokoju szafa wnękowa. 
-Pokój z kanapą narożną, TV i balkonem. Sypialnia z dużym, podwójnym łóżkiem. 
-Kuchnia z pełnym wyposażeniem: zmywarka, lodówka, piekarnik, stół śniadaniowy. Łazienka z prysznicem i pralką.
-Szybki internet 100 MB i TV satelitarna w cenie najmu! 
-Blisko Outlet Factory, Park Tysiąclecia, Port Lotniczy, Obwodnica Wrocławia. Świetnie skomunikowane - 15 min do rynku, 10 min do lotniska.
-Idealne dla pracowników lotniska i przewoźników lotniczych.
-W pobliżu przystanki komunikacji miejskiej. To przestronne, wykończone w wysokim standardzie mieszkanie doskonałe dla pary profesjonalistów lub singla.Cena najmu 2000 plus czynsz oraz zużycie gazu i prądu wg liczników, łącznie opłaty ok. 500zł. Kaucja w wysokości ceny najmu. Dostępne od września.</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/komfortowe-2-pok-internet-tv-sat-wyposazone-ul-hlaski-muchobor-CID3-IDBOLem.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>562732939</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Mieszkanie 2-pokojowe Corte Verona Grabiszyńska wyposażone</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2 000 zł</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Osoby prywatnej</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>48 m²</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>450 zł</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Krzyki</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>Do wynajęcia mieszkanie 2-pokojowe położone na strzeżonym osiedlu Corte Verona przy ul. Grabiszyńskiej. W pobliżu znajduje się m.in. market Lidl, centrum handlowe Tarasy Grabiszyńskie oraz biblioteka.
-Mieszkanie składa się z:
-- salonu połączonego z aneksem kuchennym,
-- sypialni,
-- łazienki,
-- garderoby,
-- balkonu.
-Lokal jest w pełni umeblowany, wyposażony w klimatyzację na upalne dni, a w kuchni dostępne są naczynia oraz sztućce.
-Cena: 2000 zł + opłaty ok 500 zł (czynsz do wspólnoty i prąd). Wymagana kaucja 2000 zł.
-Preferowany najem długoterminowy.
-Nie akceptujemy zwierząt.
-Możliwość oglądania mieszkania i wprowadzenia się po 1. listopada. 
-W razie pytań proszę o kontakt za pośrednictwem OLX lub SMS  502 - pokaż numer telefonu - .</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-2-pokojowe-corte-verona-grabiszynska-wyposazone-CID3-IDC5axJ.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>556935556</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Mieszkanie do wynajęcia - nowe osiedle</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>2 000 zł</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Osoby prywatnej</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>46,50 m²</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>500 zł</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Krzyki</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
         <is>
           <t>Mieszkanie w nowym budownictwie – zlokalizowane ul. Opolskiej. Doskonała oferta dla osób zainteresowanych długoterminowym wynajmem, bez ryzyka, że właściciel po kilku miesiącach wypowie umowę. Preferowane osoby niepalące (palenie wyłącznie na balkonie). 
 •	Powierzchnia: ok. 46,5 m²
@@ -2836,37 +2571,255 @@
 Ogłoszenie nie stanowi oferty w rozumieniu kodeksu cywilnego.</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/mieszkanie-do-wynajecia-nowe-osiedle-CID3-IDBGQny.html#3c151eb37f</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>562858051</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Dwupokojowe z ogrodem 50 m od parku</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2 000 zł
+Do negocjacji</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Parter</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>35 m²</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>1 zł</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Krzyki</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>października</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>2019,</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Do wynajęcia 2-pokojowe mieszkanie wraz z przynależnym ogródkiem 50 metrów od Parku Wschodniego (ul. Rybnicka) na parterze czteropiętrowego bloku. Mieszkanie jest nowe, oddane do użytku w sierpniu 2019 r., nowy lokalor będzie pierwszym najemcą. 
+Mieszkanie składa się z dwóch pokoi: salonu z aneksem kuchennym i sypialni. W kuchni znajduje się nowe AGD: lodówko-zamrażarka, piekarnik z kuchenką elektryczną, w łazience nowy prysznic z deszczownicą, WC i nową pralką, w sypialni dwuosobowe łóżko i szafa ubraniowa, w salonie dwuosobowa rozkładana sofa z TV. Całe umeblowanie mieszkania jest nowe. Mieszkanie podłączone jest do centralnego ogrzewania, a nadto aby obniżyć koszty eksploatacji na dachu bloku zamontowane zostały solary.
+Mieszkanie dostępne jest od zaraz. 
+Dojazd od mieszkania jest dobrze skomunikowany do pozostałych dzielnic Wrocławia (m.in. 10 min do Galerii Dominikańskiej, 16 min do Politechniki, 11 min do Uniwersytetu Ekonomicznego, 9 min do Uniwersyteckiego Szpitala Klinicznego). W pobliżu liczne sklepy i punkty usługowe np. Piotr i Paweł, restauracje.  
+Opłaty:
+- czynsz najmu 2000 zł/m-c
+- opłaty eksploatacyjne 400 zł m/c
+- kaucja.
+DODATKOWE INFORMACJE
+Mieszkanie idealne dla jednej osoby lub pary. Osoby niepalące, bez zwierząt. Umowa do końca września 2020 r. (z możliwym przedłużeniem).</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>883-010-777</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/dwupokojowe-z-ogrodem-50-m-od-parku-CID3-IDC5H5F.html#a4c335e894</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>562850684</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Mieszkanie 2 pokojowe na WYNAJEM 44m2 PODWYŻSZONY STANDARD</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2 100 zł</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Osoby prywatnej</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Tak</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>44 m²</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2 pokoje</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>420 zł</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Wrocław,</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Dolnośląskie,</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Śródmieście</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>października</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>2019,</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Dzień Dobry,
+od 1 listopada posiadam na wynajem mieszkanie 2pokojowe na ul Jana Czochralskiego (budynek SIENA, 2 piętro, winda).
+Mieszkanie w nowym budownictwie, oddane do użytkowania 2 lata temu. Składa się z:
+- korytarza (szafa wnękowa na wymiar)
+- łazienki (WC, wanna, umywalka +szafka umywalkowa, nowa pralka w pełnej zabudowie)
+- osobna kuchnia z oknem! (meble kuchenne na wymiar, lodówka, zmywarka, płyta indukcyjna, piekarnik, mikrofala z funkcją grilla, expres do kawy, czajnik z regulacją temperatury. Talerze, sztućce, garnki. Dodatkowo lada z dwoma krzesłami)
+- salon (stół z 4 krzesłami, narożnik, stolik kawowy, TV + szafki stojące oraz wiszące)
+- sypialnia (duża szafa w zabudowie, sofa/łóżko- do ustalenia)
+Meble wykonane z wysokiej jakości materiałów przez firmę komandor.
+Oświetlenie w salonie, sypialni i korytarzu sterowane z pilota.
+Wszystkie okna posiadają rolety dzień/noc. W sypialni oraz kuchni dodatkowo moskitiery.
+Z salonu wyjście na duży balkon (ok 6m2).
+Opcjonalnie miejsce postojowe pojedyncze
+Internet oraz TV kablowa (128 kanałów) GRATIS!
+Osoby zainteresowane zapraszam do kontaktu oraz na oględziny!</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>573 979 567</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-do-wynajecia-nowe-osiedle-CID3-IDBGQny.html#3c151eb37f</t>
+          <t>https://www.olx.pl/oferta/mieszkanie-2-pokojowe-na-wynajem-44m2-podwyzszony-standard-CID3-IDC5FaQ.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>562722961</t>
+          <t>556843150</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>New apartment near city Center</t>
+          <t>2 pokojowe / oddzielna kuchnia / obok Sky Tower / balkon</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2 100 zł</t>
+          <t>2 200 zł</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Osoby prywatnej</t>
+          <t>Biuro / Deweloper</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2876,12 +2829,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Apartamentowiec</t>
+          <t>Blok</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>38 m²</t>
+          <t>53 m²</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2891,7 +2844,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>350 zł</t>
+          <t>600 zł</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2906,7 +2859,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Śródmieście</t>
+          <t>Krzyki</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2926,43 +2879,83 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>New apartment near center available for rent now. Apartment is located in brand new building “ Krakowskie Tarasy” on Krakowska 84 street. There is tram and bus stop just in front of building, so it takes 10min to get to city center and market square. There is a lot of shops located nearby. Moreover there is plenty of waking paths and rest arena around you can relax after hours. Studio consist of 2 individual livingrooms, so can be occupied by 2 individuals or couple. Apartment is brand new and fully equipped (washing machine, microwave etc).It is located on the 9th floor with spectacular view over the city and Hala Ludowa Price: 2100 PLN plus the fees covering administrative rent, bills for water, heating, electricity verified on a monthly basis based on the real usage. Do not hesitate to contact us and see studio: Barbara:  485 - pokaż numer telefonu - 7 357Greg:  486 - pokaż numer telefonu - 6 280 This is non smoking apartment and pets are not allowed.
-~`` 
-Nowe mieszkanie blisko centrum dla dwóch osób/pary przy ul Krakowskiej dostepne od zaraz Mieszkanie znajduje sie w nowej inwestycji „Krakowskie Tarasy” przy ulicy Krakowskiej 84. Przy budynku znajduje sie przystanek tramwajowy i autobusowy. Dojazd do centrum zajmuje ok 10min tramwajem W najbliższej okolicy jest również centrum handlowe , duzo zielonych terenów nad rzeka oraz trasy spacerowe I ściezki rowerowe, Lokal ma 38m2 i składa się z dwoch niezależnych pokoi, każdy z osobnym wyjściem na taras, kuchni, łazienki I przedpokoju. Mieszkanie jest w pełni wyposażone: pralka, lodówka, mikrofala, meble. Preferowane osoby pracujące, niepalące bez zwierzat Cena: 2100.PLN za m-c plus opłaty eksploatacyjne.
-Zapraszamy do kontaktu i oglądania: Barbara:  507 - pokaż numer telefonu -  Grzegorz  607 - pokaż numer telefonu -</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr"/>
+          <t>Do wynajęcia przestronne, dwupokojowe mieszkanie z widokiem na Sky Tower, z oddzielną kuchnią, dwoma dużymi balkonami - zlokalizowane przy ul. Powstańców Śląskich obok ulicy Zaolziańskiej. Zarówno dla rodzin jak i  osób studiujących. 
+Doskonała lokalizacja: w pobliżu Pasaż Zielińskiego, Arkady Wrocławskie, Sky Tower, Galeria Wroclavia, Dworzec Autobusowy i Główny, wiele restauracji, apteka, szkoły, tereny zielone, bank, sklepy spożywcze itd. 
+Idealne połączenie z resztą miasta:
+- 7 min. do Rynku,
+- 5 min. spacerkiem do Dworca Głównego i Autobusowego oraz Galerii Wroclavia,
+- 3 min. do Arkad Wrocławskich i Galerii Handlowej Sky Tower,
+- około 15. min na Politechnikę Wrocławską i Pasażu Grunwaldzkiego,
+- 10 min. do Uniwersytetu Ekonomicznego, Wrocławskiego,
+- 20 min. do Wyższej Szkoły Bankowej i Dolnośląskiej Szkoły Wyższej.
+OPIS MIESZKANIA:
+Mieszkanie (53m2) składa się z:
+- kuchni, wyposażonej we wszystkie niezbędne sprzęty: meble, zlewozmywak, okap, kuchenka gazowa, piekarnik, nowa lodówka i zamrażarka oraz zmywarka, stól, krzesła.
+- łazienki: prysznic, umywalka, lustro, szafki, półki, nowa pralka.
+- osobnej toalety, 
+- dwóch pokoi ( 21m2 i 11m2), w których znajdują się nowe meble: łóżka dwuosobowe, komoda, stolik nocny. Możliwe domeblowanie ze strony Właściciela na życzenie najemcy. 
+- przedpokoju, w którym znajduje się duża pojemna szafa z lustrem,
+- wiatrołapu, przedsionka, również z dużą szafą,
+- balkonu 6m2.
+Dodatkowe informacje:
+Najem długoterminowy min. 1 rok. 
+Przyjazne dla zwierząt: nie
+Internet: możliwość podłączenia
+Telewizja: możliwość podłączenia
+Miejsca postojowe:  miejsce w garażu, dodatkowo płatne 300 zł lub możliwość zaparkowania przed budynkiem
+Komórka lokatorska: tak, na tym samym piętrze
+Miejsce na rowery: tak
+Ogrzewanie miejskie
+Ciepła woda: miejska
+Dwie windy w budynku
+OPŁATY: 
+2 200 zł- cena najmu 
+około 600 zł - czynsz administracyjny, w tym prąd, woda, gaz
+RAZEM: około 2 800 zł
+Kaucja: 2 800 zł.
+Na wszystkie pytania odpowiem telefonicznie, zapraszam na prezentację.
+Małgorzata Pelc
+Tel. + 485 - pokaż numer telefonu - 
+Uwaga! Prezentowane w serwisie oferty nie stanowią oferty handlowej w rozumieniu art. 66 Kodeksu Cywilnego i mogą być nieaktualne.
+NOTA PRAWNA:
+Opis oferty zawarty na stronie internetowej sporządzany jest na podstawie oględzin nieruchomości oraz informacji uzyskanych od właściciela, może podlegać aktualizacji i nie stanowi oferty określonej w art. 66 i następnych K.C.</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>577 147 947</t>
+        </is>
+      </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>https://www.olx.pl/oferta/new-apartment-near-city-center-CID3-IDC57VN.html#3c151eb37f</t>
+          <t>https://www.olx.pl/oferta/2-pokojowe-oddzielna-kuchnia-obok-sky-tower-balkon-CID3-IDBGsl8.html#a4c335e894</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>562737655</t>
+          <t>549548094</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2 pok. apartament, 47m2, balkon, Wybrzeże Reymonta, od zaraz!</t>
+          <t>Mieszkanie do wynajęcia - Promenady Wrocławskie - ul. Zakładowa</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2 200 zł</t>
+          <t>2 300 zł</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Biuro / Deweloper</t>
+          <t>Osoby prywatnej</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2977,7 +2970,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>47 m²</t>
+          <t>45 m²</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2987,7 +2980,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>410 zł</t>
+          <t>500 zł</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -3007,149 +3000,20 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>18:30,</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
       <c r="Q25" t="inlineStr">
-        <is>
-          <t>LOKALIZACJA: 
-Mieszkanie znajduje sie na 4 piętrze inwestycji Rafin – Wybrzeże Reymonta, położonej przy Odrze, blisko wałów, terenów zielonych.Osiedle jest doskonale skomunikowane z każdą częścią Wrocławia, położone tylko 3 przystanki od Rynku, 1 minutę pieszo od przystanku komunikacji miejskiej, z której odjeżdżają tramwaje 14, 15, 24 oraz autobusy 142, 253, 257, 602. 
-NIERUCHOMOŚĆ: 
-Mieszkanie usytuowane jest na 4 piętrze, skierowane na wewnętrzne patio.Całość wykończona i umeblowana z myślą o szczegółach i detalach. Mieszkanie dla osób lubiących nowoczesne, skandynawskie wnętrza, pragnących poczuć się w mieszkaniu jak u siebie w domu!:) 
-Mieszkanie składa się z salonu połączonego z aneksem kuchennym, przestronnej sypialni, dużej łazienki, osobnej praktycznej garderoby oraz balkonu.Każdy pokój posiada bezpośrednie wyjście na przestronny balkon (10m2). 
-Salon świetnie wyposażony:
-- komfortowa skandynawska sofa z funkcją spania
-- regał na książki 
- - szafki na przechowywanie i szafka pod tv
-Kuchnia w pełni wyposażona, sprzęt AGD oraz dodatkowe akcesoria kuchenne:
-- Lodówko - zamrażarka
-- Zmywarka
-- Piekarnik
-- Okap
-- Płyta Indukcyjna
-- Czajnik
-- Niezbędne naczynia oraz garnki potrzebne do indukcji 
-Przy kuchni znajduje się okrągły stół z czterema krzesłami. 
-Sypialnia wyposażona została w komfortowe i przestronne łóżko, szafę do przechowywania oraz stolik nocny.  
-Duża łazienka posiada:
-- umywalkę
-- grzejnik drabinowy 
-- toaletę podwieszaną
-- wannę z prysznicem
-- pralkę 
-- regał do przechowywania
-Dodatkowo mieszkanie posiada osobną garderobę wyposażoną w szafy oraz szuflady powierzchni 3m2. 
-Koszty wynajmu mieszkania:
-2200 PLN - Czynsz najmu (plus 2000 – jednomiesięczna, zwrotna kaucja)
-410 PLN - czynsz administracyjny z zaliczkami na wodę, ogrzewanie i media, szybki internet wliczony w cenę 
-Prąd rozliczany według zużycia (ok 50zl)
-_
-Zapraszamy na prezentację
-DOCTOR HOUSE ESTATES
-tel.  883 - pokaż numer telefonu - 
-tel:  601 - pokaż numer telefonu - 
-Zamieszczona oferta nie stanowi oferty w rozumieniu Kodeksu Cywilnego, a dane w niej zawarte mają jedynie charakter informacyjny i mogą ulec zmianie.</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/2-pok-apartament-47m2-balkon-wybrzeze-reymonta-od-zaraz-CID3-IDC5bLN.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>549548094</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Mieszkanie do wynajęcia - Promenady Wrocławskie - ul. Zakładowa</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>2 300 zł</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Osoby prywatnej</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Apartamentowiec</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>45 m²</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>500 zł</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Śródmieście</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>18:30,</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
         <is>
           <t>Wynajmę mieszkanie 2-pokojowe we Wrocławiu przy ul. Zakładowej w inwestycji Promenady Wrocławskie.
 Mieszkanie o wielkości 45m składa się z sypialni, salonu z aneksem kuchennym, łazienki, garderoby oraz balkonu. 
@@ -3165,204 +3029,95 @@
 Kaucja w wysokości 3000 zł.</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>794-140-116</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/mieszkanie-do-wynajecia-promenady-wroclawskie-ul-zakladowa-CID3-IDBbQyV.html#a4c335e894</t>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/mieszkanie-do-wynajecia-promenady-wroclawskie-ul-zakladowa-CID3-IDBbQyV.html#3c151eb37f</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>562746685</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>PIERWSZY NAJEM | 2 pokoje | NOWE | CENTRUM/Nadodrze</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>2 400 zł</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>562112416</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>LEGNICKA 2 pokoje Wysoki Standard DOSTĘPNE OD JUŻ !</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2 550 zł</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
         <is>
           <t>Biuro / Deweloper</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Apartamentowiec</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>44 m²</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Blok</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>44,02 m²</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>2 pokoje</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>400 zł</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>450 zł</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>Wrocław,</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>Dolnośląskie,</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M26" t="inlineStr">
         <is>
           <t>Śródmieście</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr">
+      <c r="N26" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="O26" t="inlineStr">
         <is>
           <t>października</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>2019,</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>ZOSTAŃ PIERWSZYM NAJEMCĄ!
-Do wynajęcia 2-pokojowe mieszkanie w okolicy ul. Pomorskiej. Nowa inwestycja!
-Lokal mieści się na IV pietrze w czteropiętrowym apartamentowcu z 2019 roku. Budynek z windą.
-Mieszkanie składa się z przestronnego, jasnego salonu z balkonem, oddzielnej sypialni oraz łazienki wanną. W budynku znajduje się dostępna dla mieszkańców rowerownia. Wszystkie media miejskie.
-Mieszkanie jest w pełni umeblowane oraz wyposażone w niezbędne sprzęty AGD
-Do wynajęcia od ZARAZ. Idealne dla pary lub singla.
-Bardzo dobra lokalizacja! Świetne połączenie komunikacją miejską z każdą częścią miasta - najbliższy przystanek: pl. Staszica. W okolicy liczne sklepy oraz kawiarnie.
-Cena: 2400 zł. + 400 zł opłaty administracyjne + prąd (około 100 zł.)
-Kaucja 2900 zł.
-Zapraszam na prezentację!
-Weronika Burlińska
-Fidom Nieruchomości
-tel.  512 - pokaż numer telefonu -</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/pierwszy-najem-2-pokoje-nowe-centrum-nadodrze-CID3-IDC5e7r.html#3c151eb37f</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>562112416</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>LEGNICKA 2 pokoje Wysoki Standard DOSTĘPNE OD JUŻ !</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>2 550 zł</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Biuro / Deweloper</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Blok</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>44,02 m²</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2 pokoje</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>450 zł</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Wrocław,</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Dolnośląskie,</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>Śródmieście</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>października</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>2019,</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
+      <c r="Q26" t="inlineStr">
         <is>
           <t>English description is below polish description + I speak english You can call me + 486 - pokaż numer telefonu -  - apartment AVAILABLE FROM NOW.
 2550 zł czynsz najmu + 450 zaliczka na poczet opłat MIESZKANIE DOSTĘPNE OD ZARAZ
@@ -3409,99 +3164,95 @@
 + 486 - pokaż numer telefonu -</t>
         </is>
       </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>502 672 328</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/legnicka-2-pokoje-wysoki-standard-dostepne-od-juz-CID3-IDC2z7i.html#a4c335e894</t>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/legnicka-2-pokoje-wysoki-standard-dostepne-od-juz-CID3-IDC2z7i.html#3c151eb37f</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>562782301</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Biskupin mieszkanie do wynajęcia ul Wiwulskiego</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>2 700 zł</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Biuro / Deweloper</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>Parter</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>Apartamentowiec</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>52 m²</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>2 pokoje</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>640 zł</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>Wrocław,</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>Dolnośląskie,</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr">
+      <c r="M27" t="inlineStr">
         <is>
           <t>Śródmieście</t>
         </is>
       </c>
-      <c r="N29" t="inlineStr">
+      <c r="N27" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
+      <c r="O27" t="inlineStr">
         <is>
           <t>października</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr">
+      <c r="P27" t="inlineStr">
         <is>
           <t>2019,</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr">
+      <c r="Q27" t="inlineStr">
         <is>
           <t>Lokal położony jest na Biskupinie w samym centrum Wrocławia- na wysokim parterze,  Budynek jest ogrodzony. 
 W pobliżu w odległości około 350 metrów są przystanki tramwajowe i autobusowe (róg ulicy Wittiga / Olszewskiego / Wróblewskiego). 
@@ -3520,99 +3271,95 @@
 tel  883 - pokaż numer telefonu -</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>883-183-900</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>https://www.olx.pl/oferta/biskupin-mieszkanie-do-wynajecia-ul-wiwulskiego-CID3-IDC5nnT.html#a4c335e894</t>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/oferta/biskupin-mieszkanie-do-wynajecia-ul-wiwulskiego-CID3-IDC5nnT.html#3c151eb37f</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
         <is>
           <t>562755002</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Przestronny apartament 2-pok. z ogrodem, Partynice</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>2 800 zł</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Biuro / Deweloper</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>Parter</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>Apartamentowiec</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>70 m²</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>2 pokoje</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>500 zł</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>Wrocław,</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>Dolnośląskie,</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="M28" t="inlineStr">
         <is>
           <t>Krzyki</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr">
+      <c r="N28" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O30" t="inlineStr">
+      <c r="O28" t="inlineStr">
         <is>
           <t>października</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr">
+      <c r="P28" t="inlineStr">
         <is>
           <t>2019,</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="Q28" t="inlineStr">
         <is>
           <t>Do wynajęcia przytulne 2-pokojowe mieszkanie z tarasem i ogrodem na Partynicach. Mieszkanie ma powierzchnie 70 m2 . Znajduje się na parterze w nowym budownictwie. Mieszkanie jest w pełni wyposażone i bardzo komfortowe. Gotowe do wprowadzenia się. Do mieszkania przynależy miejsce parkingowe.
 UKŁAD POMIESZCZEŃ:
@@ -3644,99 +3391,95 @@
 El Dorado Nieruchomości</t>
         </is>
       </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>665 631 735</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr">
         <is>
           <t>https://www.olx.pl/oferta/przestronny-apartament-2-pok-z-ogrodem-partynice-CID3-IDC5ghA.html#3c151eb37f</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
         <is>
           <t>556783567</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Wyspiańskiego 11 - Apartament na Grunwaldzkim - BEZ PROWIZJI</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>3 000 zł</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Biuro / Deweloper</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>Apartamentowiec</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>38 m²</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>2 pokoje</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>600 zł</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>Wrocław,</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>Dolnośląskie,</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr">
+      <c r="M29" t="inlineStr">
         <is>
           <t>Śródmieście</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
+      <c r="O29" t="inlineStr">
         <is>
           <t>października</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr">
+      <c r="P29" t="inlineStr">
         <is>
           <t>2019,</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr">
+      <c r="Q29" t="inlineStr">
         <is>
           <t>BEZ PROWIZJI
 Do wynajęcia mieszkanie o wysokim standardzie w apartamentowcu nad Odrą, przy Pl.Grunwaldzkim. Budynek z recepcją, sauną, siłownią, chroniony.
@@ -3760,12 +3503,8 @@
 Umowa na min.12 miesięcy. Mieszkanie dla pary lub singla, dostępne w ciągu 2-3 tygodni.</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>0048 507 00</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr">
         <is>
           <t>https://www.olx.pl/oferta/wyspianskiego-11-apartament-na-grunwaldzkim-bez-prowizji-CID3-IDBGcQ7.html#3c151eb37f</t>
         </is>

</xml_diff>